<commit_message>
Updates by MP: rm Regressed, necrotic
</commit_message>
<xml_diff>
--- a/CombinedData/MelanomaIL2_SampleAnnotations.xlsx
+++ b/CombinedData/MelanomaIL2_SampleAnnotations.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pourmalm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\HaloData\Melanoma_IL2__Final\CombinedData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5DE49F07-F593-491E-BFB9-B8B2A6CCE6A7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B2297643-97BE-4101-81CB-A608EBFEADC3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2374,6 +2374,12 @@
       <c r="X21" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="Y21" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="1">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">

</xml_diff>